<commit_message>
feat: :sparkles: ch3 processes-drivers
</commit_message>
<xml_diff>
--- a/chapter3/ch3_tables.xlsx
+++ b/chapter3/ch3_tables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songshgeo/Documents/Pycharm/HMEvolution_YRB_2022/chapter3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC064D5-6B0A-7D45-96B2-CED92BF929F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BB8419-A4AF-2C42-8784-370ED69DFF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="3440" windowWidth="28240" windowHeight="17440" activeTab="1" xr2:uid="{56C2D926-B165-2B43-BB9C-F47DC668AD86}"/>
+    <workbookView xWindow="9520" yWindow="3440" windowWidth="28240" windowHeight="17440" activeTab="2" xr2:uid="{56C2D926-B165-2B43-BB9C-F47DC668AD86}"/>
   </bookViews>
   <sheets>
     <sheet name="黄河历史时期数据来源" sheetId="1" r:id="rId1"/>
     <sheet name="影响强度半定量化" sheetId="2" r:id="rId2"/>
+    <sheet name="历史时期特征划分" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
   <si>
     <t>数据集</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,89 +187,183 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>黄河下游堤防崩溃的次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>书籍在帅王那考证一下</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结合历史地图和取样测定的黄河古河道沉积速率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沉积样本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>样本所在的古河道时间跨度越长样本越精确</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xu 2003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xu2003a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>古河道沉积速率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三门峡航运情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>强度等级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-2 cm/yr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-4 cm/yr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt; 4cm /yr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; 10次 / 20yrs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10~20次 / 20yrs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;20次 / 20yrs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自由通行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要人力辅助</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完全无法通行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>洪泛决溢频次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>历史时期黄河航运与水沙关系的研究</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>黄河流域环境变化及水沙运输规律研究文集</t>
-  </si>
-  <si>
-    <t>黄河下游堤防崩溃的次数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>书籍在帅王那考证一下</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结合历史地图和取样测定的黄河古河道沉积速率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>沉积样本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>样本所在的古河道时间跨度越长样本越精确</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Xu 2003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xu2003a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>古河道沉积速率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>三门峡航运情况</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>强度等级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0-2 cm/yr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2-4 cm/yr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt; 4cm /yr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt; 10次 / 20yrs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10~20次 / 20yrs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;20次 / 20yrs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自由通行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要人力辅助</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完全无法通行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>洪泛决溢频次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间跨度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时段划分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要特征</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200BC-400AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>400-900AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>900-1100AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1100-1350AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1350-1700AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1700-1900AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1900-2000AD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据不可信时段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>各数据集在此时期的可信度均偏低</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDP1前期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDP1时期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDP1后期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDP2前期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDP2时期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDP2时期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有明显的驱动因素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>气候驱动与低水平的人类活动驱动时期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人类活动驱动时期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>气候驱动与人类活动共同驱动时期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人口迅速增长的人类活动强烈驱动期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -276,7 +371,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -289,6 +384,14 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -341,7 +444,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -352,6 +455,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -671,7 +777,7 @@
   <dimension ref="A2:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -816,10 +922,10 @@
         <v>37</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -830,7 +936,7 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -845,7 +951,7 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -856,19 +962,19 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="G9" t="s">
         <v>44</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -882,7 +988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9988B7-2A23-5742-A207-5EC63ED0776B}">
   <dimension ref="A2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -895,16 +1001,16 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -912,13 +1018,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -926,13 +1032,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -940,13 +1046,122 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1021B03-FB0E-4643-89BE-9AE94D8F9E86}">
+  <dimension ref="A2:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>